<commit_message>
correciones cantones y nombre presidenta
</commit_message>
<xml_diff>
--- a/public/Data/datos_mujeres_presidentas.xlsx
+++ b/public/Data/datos_mujeres_presidentas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Universidad Central del Ecuador\Practicas\8.- Proyecto Identidad Rural\Datos Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danga\Downloads\ConagopareWeb\public\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD73D2A2-ACBB-4DE3-8FBF-23DF06B7FB45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1050598-C953-433B-9EF0-3B06A44E8B00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="3" r:id="rId1"/>
@@ -1985,9 +1985,6 @@
     <t>MARIA ISABEL BEJARANO YEPEZ</t>
   </si>
   <si>
-    <t>LIDA PAZ MATILDE BASTIDAS TORRES</t>
-  </si>
-  <si>
     <t>ROSA CHUQUIMARCA</t>
   </si>
   <si>
@@ -2893,6 +2890,9 @@
   </si>
   <si>
     <t>SANTO DOMINGO DE LOS TSÁCHILAS</t>
+  </si>
+  <si>
+    <t>NATHALY GALLARDO</t>
   </si>
 </sst>
 </file>
@@ -3260,8 +3260,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FD793EE-D01E-4837-9254-CC2F48CD7123}">
   <dimension ref="A1:I478"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E79" sqref="E79"/>
+    <sheetView tabSelected="1" topLeftCell="A147" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F166" sqref="F166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3270,7 +3270,7 @@
     <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="49.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4510,7 +4510,7 @@
         <v>85</v>
       </c>
       <c r="F54" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="G54" s="2">
         <v>1</v>
@@ -4602,7 +4602,7 @@
         <v>93</v>
       </c>
       <c r="F58" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="G58" s="2">
         <v>1</v>
@@ -5030,7 +5030,7 @@
         <v>350</v>
       </c>
       <c r="C77" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="D77" t="s">
         <v>122</v>
@@ -5053,7 +5053,7 @@
         <v>350</v>
       </c>
       <c r="C78" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="D78" t="s">
         <v>122</v>
@@ -5292,7 +5292,7 @@
         <v>137</v>
       </c>
       <c r="F88" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="G88" s="2">
         <v>1</v>
@@ -5450,7 +5450,7 @@
         <v>407</v>
       </c>
       <c r="E95" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="F95" t="s">
         <v>581</v>
@@ -6833,7 +6833,7 @@
         <v>93</v>
       </c>
       <c r="F155" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="G155" s="2">
         <v>1</v>
@@ -7017,7 +7017,7 @@
         <v>112</v>
       </c>
       <c r="F163" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="G163" s="2">
         <v>1</v>
@@ -7063,7 +7063,7 @@
         <v>195</v>
       </c>
       <c r="F165" t="s">
-        <v>649</v>
+        <v>951</v>
       </c>
       <c r="G165" s="2">
         <v>1</v>
@@ -7086,7 +7086,7 @@
         <v>196</v>
       </c>
       <c r="F166" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="G166" s="2">
         <v>1</v>
@@ -7109,7 +7109,7 @@
         <v>480</v>
       </c>
       <c r="F167" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="G167" s="2">
         <v>1</v>
@@ -7132,7 +7132,7 @@
         <v>197</v>
       </c>
       <c r="F168" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="G168" s="2">
         <v>1</v>
@@ -7155,7 +7155,7 @@
         <v>198</v>
       </c>
       <c r="F169" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="G169" s="2">
         <v>1</v>
@@ -7178,7 +7178,7 @@
         <v>116</v>
       </c>
       <c r="F170" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="G170" s="2">
         <v>1</v>
@@ -7201,7 +7201,7 @@
         <v>481</v>
       </c>
       <c r="F171" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="G171" s="2">
         <v>1</v>
@@ -7224,7 +7224,7 @@
         <v>482</v>
       </c>
       <c r="F172" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="G172" s="2">
         <v>1</v>
@@ -7247,7 +7247,7 @@
         <v>200</v>
       </c>
       <c r="F173" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="G173" s="2">
         <v>1</v>
@@ -7330,7 +7330,7 @@
         <v>350</v>
       </c>
       <c r="C177" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="D177" t="s">
         <v>201</v>
@@ -7339,7 +7339,7 @@
         <v>202</v>
       </c>
       <c r="F177" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="G177" s="2">
         <v>1</v>
@@ -7353,7 +7353,7 @@
         <v>350</v>
       </c>
       <c r="C178" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="D178" t="s">
         <v>122</v>
@@ -7362,7 +7362,7 @@
         <v>203</v>
       </c>
       <c r="F178" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="G178" s="2">
         <v>1</v>
@@ -7385,7 +7385,7 @@
         <v>205</v>
       </c>
       <c r="F179" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="G179" s="2">
         <v>1</v>
@@ -7408,7 +7408,7 @@
         <v>207</v>
       </c>
       <c r="F180" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="G180" s="2">
         <v>1</v>
@@ -7431,7 +7431,7 @@
         <v>210</v>
       </c>
       <c r="F181" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="G181" s="2">
         <v>1</v>
@@ -7454,7 +7454,7 @@
         <v>211</v>
       </c>
       <c r="F182" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="G182" s="2">
         <v>1</v>
@@ -7477,7 +7477,7 @@
         <v>212</v>
       </c>
       <c r="F183" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="G183" s="2">
         <v>1</v>
@@ -7500,7 +7500,7 @@
         <v>217</v>
       </c>
       <c r="F184" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="G184" s="2">
         <v>1</v>
@@ -7523,7 +7523,7 @@
         <v>213</v>
       </c>
       <c r="F185" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="G185" s="2">
         <v>1</v>
@@ -7546,7 +7546,7 @@
         <v>214</v>
       </c>
       <c r="F186" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="G186" s="2">
         <v>1</v>
@@ -7569,7 +7569,7 @@
         <v>215</v>
       </c>
       <c r="F187" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="G187" s="2">
         <v>1</v>
@@ -7592,7 +7592,7 @@
         <v>137</v>
       </c>
       <c r="F188" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="G188" s="2">
         <v>1</v>
@@ -7615,7 +7615,7 @@
         <v>24</v>
       </c>
       <c r="F189" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="G189" s="2">
         <v>1</v>
@@ -7638,7 +7638,7 @@
         <v>403</v>
       </c>
       <c r="F190" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="G190" s="2">
         <v>1</v>
@@ -7661,7 +7661,7 @@
         <v>137</v>
       </c>
       <c r="F191" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="G191" s="2">
         <v>1</v>
@@ -7684,7 +7684,7 @@
         <v>355</v>
       </c>
       <c r="F192" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="G192" s="2">
         <v>1</v>
@@ -7707,7 +7707,7 @@
         <v>356</v>
       </c>
       <c r="F193" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="G193" s="2">
         <v>1</v>
@@ -7724,13 +7724,13 @@
         <v>145</v>
       </c>
       <c r="D194" t="s">
+        <v>838</v>
+      </c>
+      <c r="E194" t="s">
         <v>839</v>
       </c>
-      <c r="E194" t="s">
+      <c r="F194" t="s">
         <v>840</v>
-      </c>
-      <c r="F194" t="s">
-        <v>841</v>
       </c>
       <c r="G194" s="2">
         <v>1</v>
@@ -7753,7 +7753,7 @@
         <v>410</v>
       </c>
       <c r="F195" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="G195" s="2">
         <v>1</v>
@@ -7776,7 +7776,7 @@
         <v>243</v>
       </c>
       <c r="F196" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="G196" s="2">
         <v>1</v>
@@ -7799,7 +7799,7 @@
         <v>24</v>
       </c>
       <c r="F197" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="G197" s="2">
         <v>1</v>
@@ -7822,7 +7822,7 @@
         <v>411</v>
       </c>
       <c r="F198" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="G198" s="2">
         <v>1</v>
@@ -7845,7 +7845,7 @@
         <v>359</v>
       </c>
       <c r="F199" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="G199" s="2">
         <v>1</v>
@@ -7868,7 +7868,7 @@
         <v>148</v>
       </c>
       <c r="F200" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="G200" s="2">
         <v>1</v>
@@ -7891,7 +7891,7 @@
         <v>78</v>
       </c>
       <c r="F201" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="G201" s="2">
         <v>1</v>
@@ -7914,7 +7914,7 @@
         <v>357</v>
       </c>
       <c r="F202" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="G202" s="2">
         <v>1</v>
@@ -7937,7 +7937,7 @@
         <v>358</v>
       </c>
       <c r="F203" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="G203" s="2">
         <v>1</v>
@@ -7960,7 +7960,7 @@
         <v>241</v>
       </c>
       <c r="F204" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="G204" s="2">
         <v>1</v>
@@ -7983,7 +7983,7 @@
         <v>360</v>
       </c>
       <c r="F205" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="G205" s="2">
         <v>1</v>
@@ -8006,7 +8006,7 @@
         <v>416</v>
       </c>
       <c r="F206" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="G206" s="2">
         <v>1</v>
@@ -8029,7 +8029,7 @@
         <v>247</v>
       </c>
       <c r="F207" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="G207" s="2">
         <v>1</v>
@@ -8052,7 +8052,7 @@
         <v>419</v>
       </c>
       <c r="F208" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="G208" s="2">
         <v>1</v>
@@ -8075,7 +8075,7 @@
         <v>432</v>
       </c>
       <c r="F209" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="G209" s="2">
         <v>1</v>
@@ -8098,7 +8098,7 @@
         <v>393</v>
       </c>
       <c r="F210" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="G210" s="2">
         <v>1</v>
@@ -8121,7 +8121,7 @@
         <v>434</v>
       </c>
       <c r="F211" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="G211" s="2">
         <v>1</v>
@@ -8144,7 +8144,7 @@
         <v>394</v>
       </c>
       <c r="F212" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="G212" s="2">
         <v>1</v>
@@ -8167,7 +8167,7 @@
         <v>167</v>
       </c>
       <c r="F213" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="G213" s="2">
         <v>1</v>
@@ -8213,7 +8213,7 @@
         <v>433</v>
       </c>
       <c r="F215" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="G215" s="2">
         <v>1</v>
@@ -8236,7 +8236,7 @@
         <v>396</v>
       </c>
       <c r="F216" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="G216" s="2">
         <v>1</v>
@@ -8259,7 +8259,7 @@
         <v>361</v>
       </c>
       <c r="F217" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="G217" s="2">
         <v>1</v>
@@ -8282,7 +8282,7 @@
         <v>278</v>
       </c>
       <c r="F218" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="G218" s="2">
         <v>1</v>
@@ -8305,7 +8305,7 @@
         <v>446</v>
       </c>
       <c r="F219" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="G219" s="2">
         <v>1</v>
@@ -8328,7 +8328,7 @@
         <v>448</v>
       </c>
       <c r="F220" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="G220" s="2">
         <v>1</v>
@@ -8351,7 +8351,7 @@
         <v>447</v>
       </c>
       <c r="F221" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="G221" s="2">
         <v>1</v>
@@ -8374,7 +8374,7 @@
         <v>450</v>
       </c>
       <c r="F222" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="G222" s="2">
         <v>1</v>
@@ -8397,7 +8397,7 @@
         <v>362</v>
       </c>
       <c r="F223" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="G223" s="2">
         <v>1</v>
@@ -8420,7 +8420,7 @@
         <v>270</v>
       </c>
       <c r="F224" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="G224" s="2">
         <v>1</v>
@@ -8443,7 +8443,7 @@
         <v>69</v>
       </c>
       <c r="F225" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="G225" s="2">
         <v>1</v>
@@ -8466,7 +8466,7 @@
         <v>489</v>
       </c>
       <c r="F226" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="G226" s="2">
         <v>1</v>
@@ -8489,7 +8489,7 @@
         <v>398</v>
       </c>
       <c r="F227" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="G227" s="2">
         <v>1</v>
@@ -8512,7 +8512,7 @@
         <v>399</v>
       </c>
       <c r="F228" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="G228" s="2">
         <v>1</v>
@@ -8558,7 +8558,7 @@
         <v>400</v>
       </c>
       <c r="F230" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="G230" s="2">
         <v>1</v>
@@ -8581,7 +8581,7 @@
         <v>64</v>
       </c>
       <c r="F231" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="G231" s="2">
         <v>1</v>
@@ -8604,7 +8604,7 @@
         <v>65</v>
       </c>
       <c r="F232" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="G232" s="2">
         <v>1</v>
@@ -8627,7 +8627,7 @@
         <v>67</v>
       </c>
       <c r="F233" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="G233" s="2">
         <v>1</v>
@@ -8650,7 +8650,7 @@
         <v>401</v>
       </c>
       <c r="F234" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="G234" s="2">
         <v>1</v>
@@ -8673,7 +8673,7 @@
         <v>402</v>
       </c>
       <c r="F235" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="G235" s="2">
         <v>1</v>
@@ -8696,7 +8696,7 @@
         <v>366</v>
       </c>
       <c r="F236" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="G236" s="2">
         <v>1</v>
@@ -8719,7 +8719,7 @@
         <v>368</v>
       </c>
       <c r="F237" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="G237" s="2">
         <v>1</v>
@@ -8742,7 +8742,7 @@
         <v>364</v>
       </c>
       <c r="F238" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="G238" s="2">
         <v>1</v>
@@ -8765,7 +8765,7 @@
         <v>371</v>
       </c>
       <c r="F239" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="G239" s="2">
         <v>1</v>
@@ -8788,7 +8788,7 @@
         <v>374</v>
       </c>
       <c r="F240" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="G240" s="2">
         <v>1</v>
@@ -8811,7 +8811,7 @@
         <v>373</v>
       </c>
       <c r="F241" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="G241" s="2">
         <v>1</v>
@@ -8834,7 +8834,7 @@
         <v>370</v>
       </c>
       <c r="F242" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="G242" s="2">
         <v>1</v>
@@ -8857,7 +8857,7 @@
         <v>455</v>
       </c>
       <c r="F243" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="G243" s="2">
         <v>1</v>
@@ -8880,7 +8880,7 @@
         <v>11</v>
       </c>
       <c r="F244" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="G244" s="2">
         <v>1</v>
@@ -8903,7 +8903,7 @@
         <v>289</v>
       </c>
       <c r="F245" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="G245" s="2">
         <v>1</v>
@@ -8926,7 +8926,7 @@
         <v>369</v>
       </c>
       <c r="F246" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="G246" s="2">
         <v>1</v>
@@ -8949,7 +8949,7 @@
         <v>459</v>
       </c>
       <c r="F247" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="G247" s="2">
         <v>1</v>
@@ -8972,7 +8972,7 @@
         <v>375</v>
       </c>
       <c r="F248" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="G248" s="2">
         <v>1</v>
@@ -8995,7 +8995,7 @@
         <v>372</v>
       </c>
       <c r="F249" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="G249" s="2">
         <v>1</v>
@@ -9018,7 +9018,7 @@
         <v>376</v>
       </c>
       <c r="F250" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="G250" s="2">
         <v>1</v>
@@ -9041,7 +9041,7 @@
         <v>377</v>
       </c>
       <c r="F251" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="G251" s="2">
         <v>1</v>
@@ -9064,7 +9064,7 @@
         <v>463</v>
       </c>
       <c r="F252" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="G252" s="2">
         <v>1</v>
@@ -9087,7 +9087,7 @@
         <v>467</v>
       </c>
       <c r="F253" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="G253" s="2">
         <v>1</v>
@@ -9110,7 +9110,7 @@
         <v>379</v>
       </c>
       <c r="F254" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="G254" s="2">
         <v>1</v>
@@ -9133,7 +9133,7 @@
         <v>305</v>
       </c>
       <c r="F255" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="G255" s="2">
         <v>1</v>
@@ -9156,7 +9156,7 @@
         <v>190</v>
       </c>
       <c r="F256" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="G256" s="2">
         <v>1</v>
@@ -9202,7 +9202,7 @@
         <v>470</v>
       </c>
       <c r="F258" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="G258" s="2">
         <v>1</v>
@@ -9225,7 +9225,7 @@
         <v>477</v>
       </c>
       <c r="F259" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="G259" s="2">
         <v>1</v>
@@ -9248,7 +9248,7 @@
         <v>478</v>
       </c>
       <c r="F260" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="G260" s="2">
         <v>1</v>
@@ -9271,7 +9271,7 @@
         <v>380</v>
       </c>
       <c r="F261" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="G261" s="2">
         <v>1</v>
@@ -9294,7 +9294,7 @@
         <v>479</v>
       </c>
       <c r="F262" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="G262" s="2">
         <v>1</v>
@@ -9317,7 +9317,7 @@
         <v>381</v>
       </c>
       <c r="F263" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="G263" s="2">
         <v>1</v>
@@ -9340,7 +9340,7 @@
         <v>382</v>
       </c>
       <c r="F264" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="G264" s="2">
         <v>1</v>
@@ -9363,7 +9363,7 @@
         <v>197</v>
       </c>
       <c r="F265" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="G265" s="2">
         <v>1</v>
@@ -9386,7 +9386,7 @@
         <v>116</v>
       </c>
       <c r="F266" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="G266" s="2">
         <v>1</v>
@@ -9409,7 +9409,7 @@
         <v>481</v>
       </c>
       <c r="F267" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="G267" s="2">
         <v>1</v>
@@ -9432,7 +9432,7 @@
         <v>384</v>
       </c>
       <c r="F268" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="G268" s="2">
         <v>1</v>
@@ -9455,7 +9455,7 @@
         <v>383</v>
       </c>
       <c r="F269" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="G269" s="2">
         <v>1</v>
@@ -9478,7 +9478,7 @@
         <v>483</v>
       </c>
       <c r="F270" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="G270" s="2">
         <v>1</v>
@@ -9492,7 +9492,7 @@
         <v>350</v>
       </c>
       <c r="C271" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="D271" t="s">
         <v>122</v>
@@ -9501,7 +9501,7 @@
         <v>203</v>
       </c>
       <c r="F271" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="G271" s="2">
         <v>1</v>
@@ -9515,7 +9515,7 @@
         <v>350</v>
       </c>
       <c r="C272" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="D272" t="s">
         <v>122</v>
@@ -9524,7 +9524,7 @@
         <v>385</v>
       </c>
       <c r="F272" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="G272" s="2">
         <v>1</v>
@@ -9541,13 +9541,13 @@
         <v>327</v>
       </c>
       <c r="D273" t="s">
+        <v>944</v>
+      </c>
+      <c r="E273" t="s">
         <v>945</v>
       </c>
-      <c r="E273" t="s">
-        <v>946</v>
-      </c>
       <c r="F273" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="G273" s="2">
         <v>1</v>
@@ -9564,13 +9564,13 @@
         <v>327</v>
       </c>
       <c r="D274" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="E274" t="s">
         <v>325</v>
       </c>
       <c r="F274" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="G274" s="2">
         <v>1</v>
@@ -9593,7 +9593,7 @@
         <v>392</v>
       </c>
       <c r="F275" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="G275" s="2">
         <v>1</v>
@@ -9616,7 +9616,7 @@
         <v>484</v>
       </c>
       <c r="F276" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="G276" s="2">
         <v>1</v>
@@ -9639,7 +9639,7 @@
         <v>211</v>
       </c>
       <c r="F277" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="G277" s="2">
         <v>1</v>
@@ -9662,7 +9662,7 @@
         <v>212</v>
       </c>
       <c r="F278" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="G278" s="2">
         <v>1</v>
@@ -9685,7 +9685,7 @@
         <v>485</v>
       </c>
       <c r="F279" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="G279" s="2">
         <v>1</v>
@@ -9708,7 +9708,7 @@
         <v>63</v>
       </c>
       <c r="F280" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="G280" s="2">
         <v>1</v>
@@ -9731,7 +9731,7 @@
         <v>387</v>
       </c>
       <c r="F281" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="G281" s="2">
         <v>1</v>
@@ -9754,7 +9754,7 @@
         <v>386</v>
       </c>
       <c r="F282" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="G282" s="2">
         <v>1</v>
@@ -9777,7 +9777,7 @@
         <v>71</v>
       </c>
       <c r="F283" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="G283" s="2">
         <v>1</v>
@@ -9800,7 +9800,7 @@
         <v>222</v>
       </c>
       <c r="F284" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="G284" s="2">
         <v>1</v>
@@ -9823,7 +9823,7 @@
         <v>223</v>
       </c>
       <c r="F285" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G285" s="2">
         <v>1</v>
@@ -9846,7 +9846,7 @@
         <v>2</v>
       </c>
       <c r="F286" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G286" s="2">
         <v>1</v>
@@ -9869,7 +9869,7 @@
         <v>218</v>
       </c>
       <c r="F287" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="G287" s="2">
         <v>1</v>
@@ -9892,7 +9892,7 @@
         <v>225</v>
       </c>
       <c r="F288" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G288" s="2">
         <v>1</v>
@@ -9915,7 +9915,7 @@
         <v>220</v>
       </c>
       <c r="F289" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="G289" s="2">
         <v>1</v>
@@ -9938,7 +9938,7 @@
         <v>221</v>
       </c>
       <c r="F290" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G290" s="2">
         <v>1</v>
@@ -9961,7 +9961,7 @@
         <v>227</v>
       </c>
       <c r="F291" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G291" s="2">
         <v>1</v>
@@ -9984,7 +9984,7 @@
         <v>228</v>
       </c>
       <c r="F292" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="G292" s="2">
         <v>1</v>
@@ -10007,7 +10007,7 @@
         <v>229</v>
       </c>
       <c r="F293" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="G293" s="2">
         <v>1</v>
@@ -10030,7 +10030,7 @@
         <v>405</v>
       </c>
       <c r="F294" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="G294" s="2">
         <v>1</v>
@@ -10053,7 +10053,7 @@
         <v>230</v>
       </c>
       <c r="F295" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="G295" s="2">
         <v>1</v>
@@ -10076,7 +10076,7 @@
         <v>231</v>
       </c>
       <c r="F296" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="G296" s="2">
         <v>1</v>
@@ -10099,7 +10099,7 @@
         <v>406</v>
       </c>
       <c r="F297" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="G297" s="2">
         <v>1</v>
@@ -10122,7 +10122,7 @@
         <v>233</v>
       </c>
       <c r="F298" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="G298" s="2">
         <v>1</v>
@@ -10142,10 +10142,10 @@
         <v>407</v>
       </c>
       <c r="E299" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="F299" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="G299" s="2">
         <v>1</v>
@@ -10168,7 +10168,7 @@
         <v>408</v>
       </c>
       <c r="F300" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="G300" s="2">
         <v>1</v>
@@ -10188,10 +10188,10 @@
         <v>17</v>
       </c>
       <c r="E301" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="F301" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G301" s="2">
         <v>1</v>
@@ -10214,7 +10214,7 @@
         <v>232</v>
       </c>
       <c r="F302" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="G302" s="2">
         <v>1</v>
@@ -10237,7 +10237,7 @@
         <v>410</v>
       </c>
       <c r="F303" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="G303" s="2">
         <v>1</v>
@@ -10260,7 +10260,7 @@
         <v>243</v>
       </c>
       <c r="F304" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="G304" s="2">
         <v>1</v>
@@ -10283,7 +10283,7 @@
         <v>20</v>
       </c>
       <c r="F305" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="G305" s="2">
         <v>1</v>
@@ -10306,7 +10306,7 @@
         <v>24</v>
       </c>
       <c r="F306" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="G306" s="2">
         <v>1</v>
@@ -10329,7 +10329,7 @@
         <v>148</v>
       </c>
       <c r="F307" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="G307" s="2">
         <v>1</v>
@@ -10352,7 +10352,7 @@
         <v>244</v>
       </c>
       <c r="F308" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="G308" s="2">
         <v>1</v>
@@ -10375,7 +10375,7 @@
         <v>236</v>
       </c>
       <c r="F309" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="G309" s="2">
         <v>1</v>
@@ -10398,7 +10398,7 @@
         <v>235</v>
       </c>
       <c r="F310" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="G310" s="2">
         <v>1</v>
@@ -10421,7 +10421,7 @@
         <v>237</v>
       </c>
       <c r="F311" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="G311" s="2">
         <v>1</v>
@@ -10444,7 +10444,7 @@
         <v>238</v>
       </c>
       <c r="F312" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="G312" s="2">
         <v>1</v>
@@ -10467,7 +10467,7 @@
         <v>413</v>
       </c>
       <c r="F313" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="G313" s="2">
         <v>1</v>
@@ -10490,7 +10490,7 @@
         <v>414</v>
       </c>
       <c r="F314" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="G314" s="2">
         <v>1</v>
@@ -10513,7 +10513,7 @@
         <v>239</v>
       </c>
       <c r="F315" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="G315" s="2">
         <v>1</v>
@@ -10536,7 +10536,7 @@
         <v>241</v>
       </c>
       <c r="F316" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="G316" s="2">
         <v>1</v>
@@ -10559,7 +10559,7 @@
         <v>246</v>
       </c>
       <c r="F317" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="G317" s="2">
         <v>1</v>
@@ -10582,7 +10582,7 @@
         <v>417</v>
       </c>
       <c r="F318" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="G318" s="2">
         <v>1</v>
@@ -10605,7 +10605,7 @@
         <v>247</v>
       </c>
       <c r="F319" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="G319" s="2">
         <v>1</v>
@@ -10628,7 +10628,7 @@
         <v>249</v>
       </c>
       <c r="F320" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="G320" s="2">
         <v>1</v>
@@ -10651,7 +10651,7 @@
         <v>250</v>
       </c>
       <c r="F321" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="G321" s="2">
         <v>1</v>
@@ -10674,7 +10674,7 @@
         <v>251</v>
       </c>
       <c r="F322" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="G322" s="2">
         <v>1</v>
@@ -10697,7 +10697,7 @@
         <v>420</v>
       </c>
       <c r="F323" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="G323" s="2">
         <v>1</v>
@@ -10720,7 +10720,7 @@
         <v>416</v>
       </c>
       <c r="F324" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="G324" s="2">
         <v>1</v>
@@ -10743,7 +10743,7 @@
         <v>421</v>
       </c>
       <c r="F325" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="G325" s="2">
         <v>1</v>
@@ -10766,7 +10766,7 @@
         <v>14</v>
       </c>
       <c r="F326" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="G326" s="2">
         <v>1</v>
@@ -10789,7 +10789,7 @@
         <v>422</v>
       </c>
       <c r="F327" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="G327" s="2">
         <v>1</v>
@@ -10812,7 +10812,7 @@
         <v>254</v>
       </c>
       <c r="F328" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="G328" s="2">
         <v>1</v>
@@ -10835,7 +10835,7 @@
         <v>455</v>
       </c>
       <c r="F329" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="G329" s="2">
         <v>1</v>
@@ -10858,7 +10858,7 @@
         <v>423</v>
       </c>
       <c r="F330" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="G330" s="2">
         <v>1</v>
@@ -10878,10 +10878,10 @@
         <v>161</v>
       </c>
       <c r="E331" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="F331" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="G331" s="2">
         <v>1</v>
@@ -10901,10 +10901,10 @@
         <v>161</v>
       </c>
       <c r="E332" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="F332" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="G332" s="2">
         <v>1</v>
@@ -10927,7 +10927,7 @@
         <v>425</v>
       </c>
       <c r="F333" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="G333" s="2">
         <v>1</v>
@@ -10947,10 +10947,10 @@
         <v>44</v>
       </c>
       <c r="E334" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="F334" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="G334" s="2">
         <v>1</v>
@@ -10970,10 +10970,10 @@
         <v>44</v>
       </c>
       <c r="E335" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="F335" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="G335" s="2">
         <v>1</v>
@@ -10996,7 +10996,7 @@
         <v>426</v>
       </c>
       <c r="F336" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="G336" s="2">
         <v>1</v>
@@ -11016,10 +11016,10 @@
         <v>44</v>
       </c>
       <c r="E337" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="F337" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="G337" s="2">
         <v>1</v>
@@ -11039,10 +11039,10 @@
         <v>46</v>
       </c>
       <c r="E338" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="F338" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="G338" s="2">
         <v>1</v>
@@ -11065,7 +11065,7 @@
         <v>427</v>
       </c>
       <c r="F339" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="G339" s="2">
         <v>1</v>
@@ -11088,7 +11088,7 @@
         <v>455</v>
       </c>
       <c r="F340" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="G340" s="2">
         <v>1</v>
@@ -11111,7 +11111,7 @@
         <v>158</v>
       </c>
       <c r="F341" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="G341" s="2">
         <v>1</v>
@@ -11134,7 +11134,7 @@
         <v>428</v>
       </c>
       <c r="F342" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="G342" s="2">
         <v>1</v>
@@ -11157,7 +11157,7 @@
         <v>429</v>
       </c>
       <c r="F343" s="5" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="G343" s="2">
         <v>1</v>
@@ -11203,7 +11203,7 @@
         <v>432</v>
       </c>
       <c r="F345" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="G345" s="2">
         <v>1</v>
@@ -11226,7 +11226,7 @@
         <v>167</v>
       </c>
       <c r="F346" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="G346" s="2">
         <v>1</v>
@@ -11249,7 +11249,7 @@
         <v>257</v>
       </c>
       <c r="F347" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="G347" s="2">
         <v>1</v>
@@ -11272,7 +11272,7 @@
         <v>433</v>
       </c>
       <c r="F348" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="G348" s="2">
         <v>1</v>
@@ -11295,7 +11295,7 @@
         <v>259</v>
       </c>
       <c r="F349" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="G349" s="2">
         <v>1</v>
@@ -11318,7 +11318,7 @@
         <v>260</v>
       </c>
       <c r="F350" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="G350" s="2">
         <v>1</v>
@@ -11341,7 +11341,7 @@
         <v>396</v>
       </c>
       <c r="F351" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="G351" s="2">
         <v>1</v>
@@ -11364,7 +11364,7 @@
         <v>436</v>
       </c>
       <c r="F352" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="G352" s="2">
         <v>1</v>
@@ -11387,7 +11387,7 @@
         <v>173</v>
       </c>
       <c r="F353" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="G353" s="2">
         <v>1</v>
@@ -11410,7 +11410,7 @@
         <v>439</v>
       </c>
       <c r="F354" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="G354" s="2">
         <v>1</v>
@@ -11433,7 +11433,7 @@
         <v>264</v>
       </c>
       <c r="F355" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="G355" s="2">
         <v>1</v>
@@ -11456,7 +11456,7 @@
         <v>263</v>
       </c>
       <c r="F356" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="G356" s="2">
         <v>1</v>
@@ -11479,7 +11479,7 @@
         <v>262</v>
       </c>
       <c r="F357" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="G357" s="2">
         <v>1</v>
@@ -11502,7 +11502,7 @@
         <v>175</v>
       </c>
       <c r="F358" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="G358" s="2">
         <v>1</v>
@@ -11525,7 +11525,7 @@
         <v>442</v>
       </c>
       <c r="F359" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="G359" s="2">
         <v>1</v>
@@ -11548,7 +11548,7 @@
         <v>448</v>
       </c>
       <c r="F360" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="G360" s="2">
         <v>1</v>
@@ -11571,7 +11571,7 @@
         <v>447</v>
       </c>
       <c r="F361" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="G361" s="2">
         <v>1</v>
@@ -11594,7 +11594,7 @@
         <v>362</v>
       </c>
       <c r="F362" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="G362" s="2">
         <v>1</v>
@@ -11617,7 +11617,7 @@
         <v>265</v>
       </c>
       <c r="F363" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="G363" s="2">
         <v>1</v>
@@ -11640,7 +11640,7 @@
         <v>270</v>
       </c>
       <c r="F364" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="G364" s="2">
         <v>1</v>
@@ -11663,7 +11663,7 @@
         <v>69</v>
       </c>
       <c r="F365" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="G365" s="2">
         <v>1</v>
@@ -11686,7 +11686,7 @@
         <v>179</v>
       </c>
       <c r="F366" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="G366" s="2">
         <v>1</v>
@@ -11709,7 +11709,7 @@
         <v>72</v>
       </c>
       <c r="F367" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="G367" s="2">
         <v>1</v>
@@ -11732,7 +11732,7 @@
         <v>398</v>
       </c>
       <c r="F368" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="G368" s="2">
         <v>1</v>
@@ -11755,7 +11755,7 @@
         <v>452</v>
       </c>
       <c r="F369" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="G369" s="2">
         <v>1</v>
@@ -11778,7 +11778,7 @@
         <v>271</v>
       </c>
       <c r="F370" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="G370" s="2">
         <v>1</v>
@@ -11801,7 +11801,7 @@
         <v>272</v>
       </c>
       <c r="F371" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="G371" s="2">
         <v>1</v>
@@ -11824,7 +11824,7 @@
         <v>453</v>
       </c>
       <c r="F372" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="G372" s="2">
         <v>1</v>
@@ -11847,7 +11847,7 @@
         <v>182</v>
       </c>
       <c r="F373" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="G373" s="2">
         <v>1</v>
@@ -11870,7 +11870,7 @@
         <v>66</v>
       </c>
       <c r="F374" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="G374" s="2">
         <v>1</v>
@@ -11893,7 +11893,7 @@
         <v>273</v>
       </c>
       <c r="F375" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="G375" s="2">
         <v>1</v>
@@ -11916,7 +11916,7 @@
         <v>274</v>
       </c>
       <c r="F376" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="G376" s="2">
         <v>1</v>
@@ -11939,7 +11939,7 @@
         <v>276</v>
       </c>
       <c r="F377" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="G377" s="2">
         <v>1</v>
@@ -11962,7 +11962,7 @@
         <v>277</v>
       </c>
       <c r="F378" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="G378" s="2">
         <v>1</v>
@@ -11985,7 +11985,7 @@
         <v>183</v>
       </c>
       <c r="F379" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="G379" s="2">
         <v>1</v>
@@ -12008,7 +12008,7 @@
         <v>278</v>
       </c>
       <c r="F380" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="G380" s="2">
         <v>1</v>
@@ -12031,7 +12031,7 @@
         <v>280</v>
       </c>
       <c r="F381" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="G381" s="2">
         <v>1</v>
@@ -12054,7 +12054,7 @@
         <v>282</v>
       </c>
       <c r="F382" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="G382" s="2">
         <v>1</v>
@@ -12077,7 +12077,7 @@
         <v>454</v>
       </c>
       <c r="F383" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="G383" s="2">
         <v>1</v>
@@ -12100,7 +12100,7 @@
         <v>284</v>
       </c>
       <c r="F384" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="G384" s="2">
         <v>1</v>
@@ -12123,7 +12123,7 @@
         <v>285</v>
       </c>
       <c r="F385" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="G385" s="2">
         <v>1</v>
@@ -12146,7 +12146,7 @@
         <v>432</v>
       </c>
       <c r="F386" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="G386" s="2">
         <v>1</v>
@@ -12169,7 +12169,7 @@
         <v>373</v>
       </c>
       <c r="F387" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="G387" s="2">
         <v>1</v>
@@ -12192,7 +12192,7 @@
         <v>287</v>
       </c>
       <c r="F388" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="G388" s="2">
         <v>1</v>
@@ -12215,7 +12215,7 @@
         <v>455</v>
       </c>
       <c r="F389" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="G389" s="2">
         <v>1</v>
@@ -12238,7 +12238,7 @@
         <v>11</v>
       </c>
       <c r="F390" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="G390" s="2">
         <v>1</v>
@@ -12261,7 +12261,7 @@
         <v>289</v>
       </c>
       <c r="F391" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="G391" s="2">
         <v>1</v>
@@ -12284,7 +12284,7 @@
         <v>85</v>
       </c>
       <c r="F392" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="G392" s="2">
         <v>1</v>
@@ -12307,7 +12307,7 @@
         <v>457</v>
       </c>
       <c r="F393" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="G393" s="2">
         <v>1</v>
@@ -12330,7 +12330,7 @@
         <v>458</v>
       </c>
       <c r="F394" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="G394" s="2">
         <v>1</v>
@@ -12353,7 +12353,7 @@
         <v>87</v>
       </c>
       <c r="F395" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="G395" s="2">
         <v>1</v>
@@ -12376,7 +12376,7 @@
         <v>459</v>
       </c>
       <c r="F396" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="G396" s="2">
         <v>1</v>
@@ -12399,7 +12399,7 @@
         <v>291</v>
       </c>
       <c r="F397" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="G397" s="2">
         <v>1</v>
@@ -12422,7 +12422,7 @@
         <v>293</v>
       </c>
       <c r="F398" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="G398" s="2">
         <v>1</v>
@@ -12445,7 +12445,7 @@
         <v>460</v>
       </c>
       <c r="F399" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="G399" s="2">
         <v>1</v>
@@ -12468,7 +12468,7 @@
         <v>249</v>
       </c>
       <c r="F400" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="G400" s="2">
         <v>1</v>
@@ -12491,7 +12491,7 @@
         <v>462</v>
       </c>
       <c r="F401" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="G401" s="2">
         <v>1</v>
@@ -12514,7 +12514,7 @@
         <v>294</v>
       </c>
       <c r="F402" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="G402" s="2">
         <v>1</v>
@@ -12537,7 +12537,7 @@
         <v>296</v>
       </c>
       <c r="F403" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="G403" s="2">
         <v>1</v>
@@ -12560,7 +12560,7 @@
         <v>298</v>
       </c>
       <c r="F404" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="G404" s="2">
         <v>1</v>
@@ -12583,7 +12583,7 @@
         <v>463</v>
       </c>
       <c r="F405" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="G405" s="2">
         <v>1</v>
@@ -12606,7 +12606,7 @@
         <v>299</v>
       </c>
       <c r="F406" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="G406" s="2">
         <v>1</v>
@@ -12629,7 +12629,7 @@
         <v>466</v>
       </c>
       <c r="F407" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="G407" s="2">
         <v>1</v>
@@ -12649,10 +12649,10 @@
         <v>465</v>
       </c>
       <c r="E408" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="F408" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="G408" s="2">
         <v>1</v>
@@ -12675,7 +12675,7 @@
         <v>95</v>
       </c>
       <c r="F409" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="G409" s="2">
         <v>1</v>
@@ -12698,7 +12698,7 @@
         <v>301</v>
       </c>
       <c r="F410" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="G410" s="2">
         <v>1</v>
@@ -12721,7 +12721,7 @@
         <v>303</v>
       </c>
       <c r="F411" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="G411" s="2">
         <v>1</v>
@@ -12744,7 +12744,7 @@
         <v>304</v>
       </c>
       <c r="F412" s="4" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="G412" s="2">
         <v>1</v>
@@ -12767,7 +12767,7 @@
         <v>305</v>
       </c>
       <c r="F413" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="G413" s="2">
         <v>1</v>
@@ -12790,7 +12790,7 @@
         <v>306</v>
       </c>
       <c r="F414" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="G414" s="2">
         <v>1</v>
@@ -12813,7 +12813,7 @@
         <v>469</v>
       </c>
       <c r="F415" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="G415" s="2">
         <v>1</v>
@@ -12836,7 +12836,7 @@
         <v>190</v>
       </c>
       <c r="F416" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="G416" s="2">
         <v>1</v>
@@ -12856,10 +12856,10 @@
         <v>104</v>
       </c>
       <c r="E417" t="s">
+        <v>928</v>
+      </c>
+      <c r="F417" t="s">
         <v>929</v>
-      </c>
-      <c r="F417" t="s">
-        <v>930</v>
       </c>
       <c r="G417" s="2">
         <v>1</v>
@@ -12882,7 +12882,7 @@
         <v>441</v>
       </c>
       <c r="F418" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="G418" s="2">
         <v>1</v>
@@ -12905,7 +12905,7 @@
         <v>307</v>
       </c>
       <c r="F419" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="G419" s="2">
         <v>1</v>
@@ -12928,7 +12928,7 @@
         <v>194</v>
       </c>
       <c r="F420" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="G420" s="2">
         <v>1</v>
@@ -12951,7 +12951,7 @@
         <v>470</v>
       </c>
       <c r="F421" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="G421" s="2">
         <v>1</v>
@@ -12974,7 +12974,7 @@
         <v>308</v>
       </c>
       <c r="F422" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="G422" s="2">
         <v>1</v>
@@ -12997,7 +12997,7 @@
         <v>471</v>
       </c>
       <c r="F423" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="G423" s="2">
         <v>1</v>
@@ -13020,7 +13020,7 @@
         <v>310</v>
       </c>
       <c r="F424" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="G424" s="2">
         <v>1</v>
@@ -13043,7 +13043,7 @@
         <v>472</v>
       </c>
       <c r="F425" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="G425" s="2">
         <v>1</v>
@@ -13066,7 +13066,7 @@
         <v>474</v>
       </c>
       <c r="F426" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="G426" s="2">
         <v>1</v>
@@ -13089,7 +13089,7 @@
         <v>475</v>
       </c>
       <c r="F427" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="G427" s="2">
         <v>1</v>
@@ -13112,7 +13112,7 @@
         <v>312</v>
       </c>
       <c r="F428" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="G428" s="2">
         <v>1</v>
@@ -13135,7 +13135,7 @@
         <v>112</v>
       </c>
       <c r="F429" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="G429" s="2">
         <v>1</v>
@@ -13158,7 +13158,7 @@
         <v>476</v>
       </c>
       <c r="F430" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="G430" s="2">
         <v>1</v>
@@ -13181,7 +13181,7 @@
         <v>478</v>
       </c>
       <c r="F431" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="G431" s="2">
         <v>1</v>
@@ -13204,7 +13204,7 @@
         <v>314</v>
       </c>
       <c r="F432" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="G432" s="2">
         <v>1</v>
@@ -13227,7 +13227,7 @@
         <v>195</v>
       </c>
       <c r="F433" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="G433" s="2">
         <v>1</v>
@@ -13250,7 +13250,7 @@
         <v>315</v>
       </c>
       <c r="F434" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="G434" s="2">
         <v>1</v>
@@ -13273,7 +13273,7 @@
         <v>197</v>
       </c>
       <c r="F435" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="G435" s="2">
         <v>1</v>
@@ -13296,7 +13296,7 @@
         <v>115</v>
       </c>
       <c r="F436" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="G436" s="2">
         <v>1</v>
@@ -13319,7 +13319,7 @@
         <v>317</v>
       </c>
       <c r="F437" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="G437" s="2">
         <v>1</v>
@@ -13342,7 +13342,7 @@
         <v>120</v>
       </c>
       <c r="F438" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="G438" s="2">
         <v>1</v>
@@ -13365,7 +13365,7 @@
         <v>483</v>
       </c>
       <c r="F439" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="G439" s="2">
         <v>1</v>
@@ -13379,7 +13379,7 @@
         <v>350</v>
       </c>
       <c r="C440" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="D440" t="s">
         <v>201</v>
@@ -13388,7 +13388,7 @@
         <v>318</v>
       </c>
       <c r="F440" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="G440" s="2">
         <v>1</v>
@@ -13402,7 +13402,7 @@
         <v>350</v>
       </c>
       <c r="C441" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="D441" t="s">
         <v>122</v>
@@ -13411,7 +13411,7 @@
         <v>319</v>
       </c>
       <c r="F441" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="G441" s="2">
         <v>1</v>
@@ -13425,7 +13425,7 @@
         <v>350</v>
       </c>
       <c r="C442" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="D442" t="s">
         <v>122</v>
@@ -13434,7 +13434,7 @@
         <v>385</v>
       </c>
       <c r="F442" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="G442" s="2">
         <v>1</v>
@@ -13448,7 +13448,7 @@
         <v>350</v>
       </c>
       <c r="C443" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="D443" t="s">
         <v>122</v>
@@ -13457,7 +13457,7 @@
         <v>320</v>
       </c>
       <c r="F443" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="G443" s="2">
         <v>1</v>
@@ -13480,7 +13480,7 @@
         <v>205</v>
       </c>
       <c r="F444" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="G444" s="2">
         <v>1</v>
@@ -13503,7 +13503,7 @@
         <v>322</v>
       </c>
       <c r="F445" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="G445" s="2">
         <v>1</v>
@@ -13526,7 +13526,7 @@
         <v>323</v>
       </c>
       <c r="F446" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="G446" s="2">
         <v>1</v>
@@ -13549,7 +13549,7 @@
         <v>325</v>
       </c>
       <c r="F447" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="G447" s="2">
         <v>1</v>
@@ -13572,7 +13572,7 @@
         <v>326</v>
       </c>
       <c r="F448" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="G448" s="2">
         <v>1</v>
@@ -13595,7 +13595,7 @@
         <v>328</v>
       </c>
       <c r="F449" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="G449" s="2">
         <v>1</v>
@@ -13618,7 +13618,7 @@
         <v>331</v>
       </c>
       <c r="F450" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="G450" s="2">
         <v>1</v>
@@ -13641,7 +13641,7 @@
         <v>332</v>
       </c>
       <c r="F451" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="G451" s="2">
         <v>1</v>
@@ -13664,7 +13664,7 @@
         <v>333</v>
       </c>
       <c r="F452" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="G452" s="2">
         <v>1</v>
@@ -13687,7 +13687,7 @@
         <v>334</v>
       </c>
       <c r="F453" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="G453" s="2">
         <v>1</v>
@@ -13711,7 +13711,7 @@
         <v>335</v>
       </c>
       <c r="F454" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="G454" s="2">
         <v>1</v>
@@ -13734,7 +13734,7 @@
         <v>336</v>
       </c>
       <c r="F455" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="G455" s="2">
         <v>1</v>
@@ -13757,7 +13757,7 @@
         <v>337</v>
       </c>
       <c r="F456" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="G456" s="2">
         <v>1</v>
@@ -13780,7 +13780,7 @@
         <v>485</v>
       </c>
       <c r="F457" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="G457" s="2">
         <v>1</v>
@@ -13803,7 +13803,7 @@
         <v>338</v>
       </c>
       <c r="F458" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="G458" s="2">
         <v>1</v>
@@ -13826,7 +13826,7 @@
         <v>339</v>
       </c>
       <c r="F459" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="G459" s="2">
         <v>1</v>
@@ -13849,7 +13849,7 @@
         <v>217</v>
       </c>
       <c r="F460" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="G460" s="2">
         <v>1</v>
@@ -13872,7 +13872,7 @@
         <v>487</v>
       </c>
       <c r="F461" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="G461" s="2">
         <v>1</v>
@@ -13895,7 +13895,7 @@
         <v>341</v>
       </c>
       <c r="F462" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="G462" s="2">
         <v>1</v>
@@ -13918,7 +13918,7 @@
         <v>343</v>
       </c>
       <c r="F463" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="G463" s="2">
         <v>1</v>
@@ -13941,7 +13941,7 @@
         <v>129</v>
       </c>
       <c r="F464" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="G464" s="2">
         <v>1</v>
@@ -13964,7 +13964,7 @@
         <v>71</v>
       </c>
       <c r="F465" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="G465" s="2">
         <v>1</v>

</xml_diff>